<commit_message>
Authentication with JWT has been implemented
</commit_message>
<xml_diff>
--- a/backend/exports/redx_export_q_Pune.xlsx
+++ b/backend/exports/redx_export_q_Pune.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2025-06-30 17:38:46</t>
+          <t>2025-07-10 11:36:59</t>
         </is>
       </c>
     </row>
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pune</t>
+          <t>PUne</t>
         </is>
       </c>
     </row>
@@ -520,27 +520,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afsar Khan</t>
+          <t xml:space="preserve"> Afsar</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>REDX_VMS Portal</t>
+          <t xml:space="preserve"> REDX</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pune, Maharashtra</t>
+          <t xml:space="preserve"> Pune</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Mr.Gagan</t>
+          <t xml:space="preserve"> Mr.Sachin</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-06-30 05:41:31</t>
+          <t>2025-07-10 05:40:09</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -570,13 +570,11 @@
       <c r="L5" t="n">
         <v>1</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="M5" t="n">
+        <v>4.17</v>
       </c>
       <c r="N5" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6">
@@ -592,17 +590,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pune, Maharashtra</t>
+          <t>Pune, Maharashtra India</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mr.Gagan</t>
+          <t>Mr.Sahil</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-06-30 05:34:04</t>
+          <t>2025-06-30 13:24:28</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -612,7 +610,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>5MP (2560x1920)</t>
+          <t>12MP (4000x3000)</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -624,21 +622,139 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="K6" t="n">
         <v>30</v>
       </c>
       <c r="L6" t="n">
+        <v>99</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1421.35</v>
+      </c>
+      <c r="N6" t="n">
+        <v>460.52</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Pune, Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Mr.Sahil</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-06-30 13:24:28</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>25</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
         <v>1</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N6" t="n">
-        <v>0.01</v>
+      <c r="K7" t="n">
+        <v>30</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1421.35</v>
+      </c>
+      <c r="N7" t="n">
+        <v>460.52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Pune, Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Mr.Sahil</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-06-30 13:24:28</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>30</v>
+      </c>
+      <c r="L8" t="n">
+        <v>42</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1421.35</v>
+      </c>
+      <c r="N8" t="n">
+        <v>460.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>